<commit_message>
Backup QR Scanner data - 04/05/2025, 3:59:37 PM
</commit_message>
<xml_diff>
--- a/backups/Scanner_Anatomy_Lecture_Hall_2025-05-04T12-45-06.xlsx
+++ b/backups/Scanner_Anatomy_Lecture_Hall_2025-05-04T12-45-06.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Anatomy_Lecture_Hall" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -416,7 +416,7 @@
         <v>Log Time</v>
       </c>
       <c r="E1" t="str">
-        <v>Type</v>
+        <v>Number</v>
       </c>
     </row>
     <row r="2">
@@ -427,13 +427,13 @@
         <v>Anatomy Lecture Hall</v>
       </c>
       <c r="C2" t="str">
-        <v>05/04/2025</v>
+        <v>04/05/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>3:45 PM</v>
+        <v>15:45:09</v>
       </c>
       <c r="E2" t="str">
-        <v>Manual</v>
+        <v>1746362709541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>